<commit_message>
OCE-5 - touched ocvn files that were deleted in oc-explorer.
</commit_message>
<xml_diff>
--- a/forms/src/main/java/org/devgateway/ocvn/forms/xlsx/Location_Table_SO.xlsx
+++ b/forms/src/main/java/org/devgateway/ocvn/forms/xlsx/Location_Table_SO.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ionut/work/ocvn/forms/src/main/java/org/devgateway/ocvn/forms/xlsx/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -598,12 +606,12 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +642,7 @@
         <v>1581188</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -780,163 +788,163 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="3"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="3"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="3"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="3"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="3"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="2"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="3"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="3"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="3"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -944,10 +952,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>